<commit_message>
Apply button is now working properly, Motor Tuned with For Resp 30 and 25 and Tidal 700
</commit_message>
<xml_diff>
--- a/docs/TdialAndDegree.xlsx
+++ b/docs/TdialAndDegree.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EVent-ir\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E163EBB-79EC-4769-A221-3640ABBFA073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D111E758-89DD-4306-BADB-4F506C4665C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6EFF8996-5790-4D37-A43C-47C8F19DF120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6EFF8996-5790-4D37-A43C-47C8F19DF120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,8 +47,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7FD53F-604A-4C0D-86FD-1955FCEA6D71}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -501,4 +511,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07439B6D-2398-4D2C-AE48-61BBAE913762}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tidal 700 Resp 15,20,25,30, IE 2 Finished, TDV Setup=MHG Inovation
</commit_message>
<xml_diff>
--- a/docs/TdialAndDegree.xlsx
+++ b/docs/TdialAndDegree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EVent-ir\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D111E758-89DD-4306-BADB-4F506C4665C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761FCF00-6BD9-456C-BD97-030857273383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6EFF8996-5790-4D37-A43C-47C8F19DF120}"/>
   </bookViews>
@@ -515,47 +515,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07439B6D-2398-4D2C-AE48-61BBAE913762}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.15</v>
+      </c>
+      <c r="B7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-6</v>
+      </c>
+      <c r="B8">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-2</v>
+      </c>
+      <c r="B9">
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuning System for TDV=300, IE 2
</commit_message>
<xml_diff>
--- a/docs/TdialAndDegree.xlsx
+++ b/docs/TdialAndDegree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EVent-ir\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761FCF00-6BD9-456C-BD97-030857273383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52C48A8-2CEF-4A05-9BCA-44AE1CC2657F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6EFF8996-5790-4D37-A43C-47C8F19DF120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6EFF8996-5790-4D37-A43C-47C8F19DF120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7FD53F-604A-4C0D-86FD-1955FCEA6D71}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07439B6D-2398-4D2C-AE48-61BBAE913762}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +536,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>